<commit_message>
Oppdatert excel-ark med logg: AdminKontoController fanen. Oppdatert navn på test-case i SoapUI.
</commit_message>
<xml_diff>
--- a/Test-Plan-Nettbank.xlsx
+++ b/Test-Plan-Nettbank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\IdeaProjects\ADTS2310-Nettbank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D756363-3C56-462B-9F84-1D720B5B268D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0A2E4E-E19E-42CE-8F39-85B6F37C858D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="30" windowWidth="27015" windowHeight="15975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oversikt" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="209">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>Search and add new customers to the system</t>
-  </si>
-  <si>
     <t>Search for existing customer by phone number</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>SoapUI</t>
   </si>
   <si>
-    <t>Logget inn, hente konto, hente saldi, endre info, betale</t>
-  </si>
-  <si>
     <t>initDB</t>
   </si>
   <si>
@@ -498,9 +492,6 @@
     <t>18-02-22 kl 11:30</t>
   </si>
   <si>
-    <t>18-02-22 kl 11:35</t>
-  </si>
-  <si>
     <t>Logget inn som "Lene Jensen"</t>
   </si>
   <si>
@@ -534,12 +525,6 @@
     <t>305010123456</t>
   </si>
   <si>
-    <t>Json objekt istedenfor parametre enkeltvis, registrerer ny konto</t>
-  </si>
-  <si>
-    <t>slettet Konto2</t>
-  </si>
-  <si>
     <t>Json objekt istedenfor parametre enkeltvis (endret saldo på nyopprettet Konto2: 5250 til 7000 NOK)</t>
   </si>
   <si>
@@ -558,9 +543,6 @@
     <t>Logget inn - Kunde</t>
   </si>
   <si>
-    <t>registrerKonto - RegEx test</t>
-  </si>
-  <si>
     <t>Json objekt istedenfor parametre enkeltvis, endrer kontonummer med over 11 siffer</t>
   </si>
   <si>
@@ -574,6 +556,111 @@
   </si>
   <si>
     <t>4. Når man er logget inn som admin med admin passord og brukernavn så sjekkes det for personnummer når man gjør ulike funksjoner som registrer() og hentAlleKoni() eks. Er det riktig?</t>
+  </si>
+  <si>
+    <t>Json objekt istedenfor parametre enkeltvis, registrerer ny konto "305010123456"</t>
+  </si>
+  <si>
+    <t>Legg til scenarioer her...</t>
+  </si>
+  <si>
+    <t>10234.5</t>
+  </si>
+  <si>
+    <t>slettet det nye kontonr, Konto2: 305010123456</t>
+  </si>
+  <si>
+    <t>16-02-22 kl 20:20</t>
+  </si>
+  <si>
+    <t>18-02-22 kl 11:25</t>
+  </si>
+  <si>
+    <t>18-02-22 kl 11:20</t>
+  </si>
+  <si>
+    <t>registrerKonto - RegEx test personnummer</t>
+  </si>
+  <si>
+    <t>registrerKonto - RegEx test kontonummer</t>
+  </si>
+  <si>
+    <t>AC-0031</t>
+  </si>
+  <si>
+    <t>AC-0032</t>
+  </si>
+  <si>
+    <t>AC-0033</t>
+  </si>
+  <si>
+    <t>AC-0034</t>
+  </si>
+  <si>
+    <t>AC-0035</t>
+  </si>
+  <si>
+    <t>AC-0036</t>
+  </si>
+  <si>
+    <t>AC-0037</t>
+  </si>
+  <si>
+    <t>AC-0039</t>
+  </si>
+  <si>
+    <t>AC-0040</t>
+  </si>
+  <si>
+    <t>AC-0041</t>
+  </si>
+  <si>
+    <t>AC-0042</t>
+  </si>
+  <si>
+    <t>AC-0043</t>
+  </si>
+  <si>
+    <t>18-02-22 kl 11:40</t>
+  </si>
+  <si>
+    <t>loggUt - Admin</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:00</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:05</t>
+  </si>
+  <si>
+    <t>loggUt - Kunde</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:10</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:15</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:20</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:25</t>
+  </si>
+  <si>
+    <t>19-02-22 kl 12:40</t>
+  </si>
+  <si>
+    <t>Ikke innlogget???</t>
+  </si>
+  <si>
+    <t>Testscenario for Admin bruker, Kunde bruker og "Ikke logget inn".</t>
+  </si>
+  <si>
+    <t>Testet mot konto innlogg, registrer, hent, endre, slett, regEx og logg ut.</t>
   </si>
 </sst>
 </file>
@@ -583,7 +670,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,6 +791,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -774,7 +869,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -841,6 +936,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
@@ -851,7 +949,296 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="132">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1585,79 +1972,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A14:C17" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A14:C17" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Testresultat Sammendrag (automatisk)" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nummer" dataDxfId="94">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Testresultat Sammendrag (automatisk)" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nummer" dataDxfId="128">
       <calculatedColumnFormula>SUM(AdminKontoController!D2,AdminKundeController!D2,BankController!D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prosent" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prosent" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table7" displayName="Table7" ref="A4:C11" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table7" displayName="Table7" ref="A4:C11" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
   <autoFilter ref="A4:C11" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Endringslogg" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Person" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Dato" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Endringslogg" dataDxfId="124"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Person" dataDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Dato" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="A8:I48" totalsRowShown="0" dataDxfId="87">
-  <autoFilter ref="A8:I48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="A9:I56" totalsRowShown="0" dataDxfId="121">
+  <autoFilter ref="A9:I56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Test Case ID" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Test Case Beskrivelse" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Forventet Resultat" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Test Data" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Faktisk Resultat" dataDxfId="82"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Status" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Testperson" dataDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Dato/Tid" dataDxfId="79"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Kommentarer" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Test Case ID" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Test Case Beskrivelse" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Forventet Resultat" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Test Data" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Faktisk Resultat" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Status" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Testperson" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Dato/Tid" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Kommentarer" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B1D577C-F950-4C9F-A60C-BB249F891B0C}" name="Table13" displayName="Table13" ref="A8:I34" totalsRowShown="0" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B1D577C-F950-4C9F-A60C-BB249F891B0C}" name="Table13" displayName="Table13" ref="A8:I34" totalsRowShown="0" dataDxfId="111">
   <autoFilter ref="A8:I34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DF416966-7C79-49CF-9C16-FF292C744D93}" name="Test Case ID" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{1609E40A-7A01-4E47-9FB5-30EE0C0100D1}" name="Test Case Beskrivelse" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{52D88C38-FADC-4958-8388-A181E397952C}" name="Forventet Resultat" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{3E2ED67D-9DBE-4BCA-A31F-05E4F7BEA8A4}" name="Test Data" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{1BA2EB1B-B994-4EA5-A612-7E54C5D6C482}" name="Faktisk Resultat" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{A8EA8379-640E-4136-86EA-8EAB6AE3D081}" name="Status" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{95F0EE31-A394-4ADD-BD55-D505F6BF1957}" name="Testperson" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{6F6461F6-7E20-4C11-A3A7-18FC4D3EC284}" name="Dato/Tid" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{40D4757F-BEFB-4F57-87EF-B57C21BD8635}" name="Kommentarer" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{DF416966-7C79-49CF-9C16-FF292C744D93}" name="Test Case ID" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{1609E40A-7A01-4E47-9FB5-30EE0C0100D1}" name="Test Case Beskrivelse" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{52D88C38-FADC-4958-8388-A181E397952C}" name="Forventet Resultat" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{3E2ED67D-9DBE-4BCA-A31F-05E4F7BEA8A4}" name="Test Data" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{1BA2EB1B-B994-4EA5-A612-7E54C5D6C482}" name="Faktisk Resultat" dataDxfId="106"/>
+    <tableColumn id="6" xr3:uid="{A8EA8379-640E-4136-86EA-8EAB6AE3D081}" name="Status" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{95F0EE31-A394-4ADD-BD55-D505F6BF1957}" name="Testperson" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{6F6461F6-7E20-4C11-A3A7-18FC4D3EC284}" name="Dato/Tid" dataDxfId="103"/>
+    <tableColumn id="9" xr3:uid="{40D4757F-BEFB-4F57-87EF-B57C21BD8635}" name="Kommentarer" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{243C7D70-44E9-4D64-A835-F96128025DB3}" name="Table134" displayName="Table134" ref="A8:I38" totalsRowShown="0" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{243C7D70-44E9-4D64-A835-F96128025DB3}" name="Table134" displayName="Table134" ref="A8:I38" totalsRowShown="0" dataDxfId="101">
   <autoFilter ref="A8:I38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9DAC78F6-778A-4FD3-877A-732350927B61}" name="Test Case ID" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{90CA3DBF-11C8-4E4A-B3F0-B8FCF2657DAE}" name="Test Case Beskrivelse" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{8BA58222-C440-4254-B982-A649C9258B69}" name="Forventet Resultat" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{A00FE3D8-76DD-4B50-B65D-2099CCA67C55}" name="Test Data" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{37947F04-D754-4B18-9FEF-E34E7251D719}" name="Faktisk Resultat" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{EEFC8D78-A622-4872-B051-A29409D18833}" name="Status" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{11CB59D7-43CB-4D3B-A142-298243ADDEAD}" name="Testperson" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{26356E35-12A7-4A0B-AEEF-0CEFF65B5C96}" name="Dato/Tid" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{F2A0BD80-F2E1-43D9-8F01-74B5AC7C28C8}" name="Kommentarer" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{9DAC78F6-778A-4FD3-877A-732350927B61}" name="Test Case ID" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{90CA3DBF-11C8-4E4A-B3F0-B8FCF2657DAE}" name="Test Case Beskrivelse" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{8BA58222-C440-4254-B982-A649C9258B69}" name="Forventet Resultat" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{A00FE3D8-76DD-4B50-B65D-2099CCA67C55}" name="Test Data" dataDxfId="97"/>
+    <tableColumn id="5" xr3:uid="{37947F04-D754-4B18-9FEF-E34E7251D719}" name="Faktisk Resultat" dataDxfId="96"/>
+    <tableColumn id="6" xr3:uid="{EEFC8D78-A622-4872-B051-A29409D18833}" name="Status" dataDxfId="95"/>
+    <tableColumn id="7" xr3:uid="{11CB59D7-43CB-4D3B-A142-298243ADDEAD}" name="Testperson" dataDxfId="94"/>
+    <tableColumn id="8" xr3:uid="{26356E35-12A7-4A0B-AEEF-0CEFF65B5C96}" name="Dato/Tid" dataDxfId="93"/>
+    <tableColumn id="9" xr3:uid="{F2A0BD80-F2E1-43D9-8F01-74B5AC7C28C8}" name="Kommentarer" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2004,7 +2391,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2012,24 +2399,24 @@
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="13">
         <v>44606</v>
@@ -2045,10 +2432,10 @@
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="13">
         <v>44609</v>
@@ -2064,10 +2451,10 @@
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="13">
         <v>44609</v>
@@ -2083,10 +2470,10 @@
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="13">
         <v>44610</v>
@@ -2133,7 +2520,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2148,13 +2535,13 @@
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -2167,15 +2554,15 @@
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="10">
         <f>SUM(AdminKontoController!D2,AdminKundeController!D2,BankController!D2)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C15" s="11">
         <f>B15/SUM(B15:B17)</f>
-        <v>0.36046511627906974</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
@@ -2188,15 +2575,15 @@
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="10">
-        <f>SUM(AdminKontoController!D3,AdminKundeController!D3,BankController!D3)</f>
-        <v>3</v>
+        <f>SUM(AdminKontoController!D4,AdminKundeController!D3,BankController!D3)</f>
+        <v>5</v>
       </c>
       <c r="C16" s="11">
         <f>B16/SUM(B15:B17)</f>
-        <v>3.4883720930232558E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -2209,15 +2596,15 @@
     </row>
     <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="10">
-        <f>SUM(AdminKontoController!D4,AdminKundeController!D4,BankController!D4)</f>
-        <v>52</v>
+        <f>SUM(AdminKontoController!D5,AdminKundeController!D4,BankController!D4)</f>
+        <v>41</v>
       </c>
       <c r="C17" s="11">
         <f>B17/SUM(B15:B17)</f>
-        <v>0.60465116279069764</v>
+        <v>0.51249999999999996</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
@@ -2251,12 +2638,12 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E22" s="29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -2328,22 +2715,22 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2365,17 +2752,17 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -2386,13 +2773,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="8"/>
     </row>
@@ -2401,145 +2788,127 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>81</v>
+        <v>207</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5">
         <f>COUNTIF(F:F,"Pass")</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="5">
-        <f>COUNTIF(F:F,"Fail")</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>73</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5">
+        <f>COUNTIF(F:F,"Fail")</f>
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="D5" s="5">
         <f>COUNTIF(F:F,"Not Started")</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
         <v>75</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>76</v>
       </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H9" t="s">
         <v>77</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I9" t="s">
         <v>78</v>
       </c>
-      <c r="I8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -2548,60 +2917,68 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="18">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="18">
-        <v>3</v>
+        <v>87</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="19" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="18">
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="E13" s="18">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>162</v>
+      <c r="C14" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2610,17 +2987,17 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" t="s">
-        <v>99</v>
+        <v>159</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2628,804 +3005,958 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25">
         <v>10234.5</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="D17" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="25">
         <v>10234.5</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="B18" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C18" s="18">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="18">
-        <v>4</v>
+        <v>88</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>165</v>
       </c>
+      <c r="C19" s="18">
+        <v>4</v>
+      </c>
       <c r="D19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="E19" s="18">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>11</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>168</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="18">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="18">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25">
-        <v>7000</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="E22" s="25">
-        <v>7000</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="24"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="B24" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C24" s="18">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="18">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>156</v>
+        <v>171</v>
+      </c>
+      <c r="C25" s="18">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="18">
+        <v>4</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>153</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25">
+        <v>7000</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="25">
+        <v>7000</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="19">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="19">
-        <v>3</v>
+        <v>108</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>156</v>
+        <v>166</v>
+      </c>
+      <c r="C31" s="18">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="18">
+        <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="21" t="s">
-        <v>157</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="21"/>
+      <c r="A32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="22"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="21"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I36" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="C37" s="18">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>114</v>
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>93</v>
       </c>
       <c r="E37" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>116</v>
+        <v>29</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="D40" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="F41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="20"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="19"/>
+        <v>184</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="F44" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="19"/>
+        <v>185</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>92</v>
+      </c>
       <c r="F45" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="19"/>
+        <v>186</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="19">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="19">
+        <v>3</v>
+      </c>
       <c r="F46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>201</v>
+      </c>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="19"/>
+        <v>187</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>91</v>
+      </c>
       <c r="F47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I48" s="21"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
+      <c r="A50" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I50" s="21"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="A52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="A53" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="18">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="18">
+        <v>0</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="A54" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
+      <c r="A55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="A56" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3527,114 +4058,338 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
-  <conditionalFormatting sqref="A9:I17 A19:I20 A23:I23 A21 A24:A26 A27:I48">
-    <cfRule type="expression" dxfId="57" priority="87">
-      <formula>$F9="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="88">
-      <formula>$F9="Pass"</formula>
+  <conditionalFormatting sqref="A10:I18 A30:I30 A26:I26 H31:H34 A20:I24 B27:I28 A25:A29 A31:A42 A43:I45 A46:G49 H46:I50 A51:I56">
+    <cfRule type="expression" dxfId="91" priority="133">
+      <formula>$F10="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="134">
+      <formula>$F10="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F42">
-    <cfRule type="expression" dxfId="55" priority="77">
-      <formula>$F41="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="78">
-      <formula>$F41="Pass"</formula>
+  <conditionalFormatting sqref="A43:I43">
+    <cfRule type="expression" dxfId="89" priority="89">
+      <formula>$F43="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="90">
+      <formula>$F43="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="53" priority="55">
-      <formula>$F41="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="56">
-      <formula>$F41="Pass"</formula>
+  <conditionalFormatting sqref="F44">
+    <cfRule type="expression" dxfId="87" priority="71">
+      <formula>$F44="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="72">
+      <formula>$F44="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:I27">
-    <cfRule type="expression" dxfId="51" priority="43">
-      <formula>$F27="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="44">
-      <formula>$F27="Pass"</formula>
+  <conditionalFormatting sqref="A19:I19">
+    <cfRule type="expression" dxfId="85" priority="57">
+      <formula>$F19="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="58">
+      <formula>$F19="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="49" priority="25">
-      <formula>$F28="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="26">
-      <formula>$F28="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36:A40">
-    <cfRule type="expression" dxfId="47" priority="17">
-      <formula>$F36="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="18">
-      <formula>$F36="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36:A40">
-    <cfRule type="expression" dxfId="45" priority="15">
-      <formula>$F36="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="16">
-      <formula>$F36="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:I18">
-    <cfRule type="expression" dxfId="43" priority="11">
-      <formula>$F18="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="12">
-      <formula>$F18="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:I24">
-    <cfRule type="expression" dxfId="41" priority="9">
-      <formula>$F24="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="10">
-      <formula>$F24="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:I21">
-    <cfRule type="expression" dxfId="39" priority="7">
-      <formula>$F21="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="8">
-      <formula>$F21="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22:I22">
-    <cfRule type="expression" dxfId="37" priority="5">
-      <formula>$F22="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="6">
-      <formula>$F22="Pass"</formula>
+  <conditionalFormatting sqref="B31:F31 I31:I34 B32:B34 F32:F34">
+    <cfRule type="expression" dxfId="83" priority="55">
+      <formula>$F31="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="56">
+      <formula>$F31="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:I25">
+    <cfRule type="expression" dxfId="81" priority="53">
+      <formula>$F25="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="54">
+      <formula>$F25="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:I29">
+    <cfRule type="expression" dxfId="79" priority="51">
+      <formula>$F29="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="52">
+      <formula>$F29="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:F35 I35">
+    <cfRule type="expression" dxfId="77" priority="49">
+      <formula>$F35="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="50">
+      <formula>$F35="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:F36 I36:I42 B42:F42 B38:B41 D41 F38:F41">
+    <cfRule type="expression" dxfId="75" priority="47">
+      <formula>$F36="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="48">
+      <formula>$F36="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31:G34">
+    <cfRule type="expression" dxfId="73" priority="45">
+      <formula>$F31="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="46">
+      <formula>$F31="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:E32">
+    <cfRule type="expression" dxfId="71" priority="43">
+      <formula>$F32="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="44">
+      <formula>$F32="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:E34">
+    <cfRule type="expression" dxfId="69" priority="41">
+      <formula>$F33="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="42">
+      <formula>$F33="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="expression" dxfId="67" priority="39">
+      <formula>$F35="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="40">
+      <formula>$F35="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36 G38:G40 G42">
+    <cfRule type="expression" dxfId="65" priority="37">
+      <formula>$F36="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="38">
+      <formula>$F36="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="63" priority="35">
+      <formula>$F35="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="36">
+      <formula>$F35="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:H40 H42">
+    <cfRule type="expression" dxfId="61" priority="33">
+      <formula>$F36="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="34">
+      <formula>$F36="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" dxfId="59" priority="31">
+      <formula>$F37="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="32">
+      <formula>$F37="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:F37">
+    <cfRule type="expression" dxfId="57" priority="27">
+      <formula>$F37="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="28">
+      <formula>$F37="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="expression" dxfId="55" priority="25">
+      <formula>$F37="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="26">
+      <formula>$F37="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:E38">
+    <cfRule type="expression" dxfId="53" priority="23">
+      <formula>$F38="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="24">
+      <formula>$F38="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:E40">
+    <cfRule type="expression" dxfId="51" priority="21">
+      <formula>$F39="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="22">
+      <formula>$F39="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="expression" dxfId="49" priority="19">
+      <formula>$F41="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="20">
+      <formula>$F41="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="expression" dxfId="47" priority="17">
+      <formula>$F41="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="18">
+      <formula>$F41="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="expression" dxfId="45" priority="15">
+      <formula>$F50="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="16">
+      <formula>$F50="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50 D50 F50">
+    <cfRule type="expression" dxfId="43" priority="13">
+      <formula>$F50="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="14">
+      <formula>$F50="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
+    <cfRule type="expression" dxfId="41" priority="11">
+      <formula>$F50="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="12">
+      <formula>$F50="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="39" priority="9">
+      <formula>$F41="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="10">
+      <formula>$F41="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="expression" dxfId="37" priority="5">
+      <formula>$F41="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="6">
+      <formula>$F41="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
     <cfRule type="expression" dxfId="35" priority="3">
-      <formula>$F25="Fail"</formula>
+      <formula>$F50="Fail"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="4">
-      <formula>$F25="Pass"</formula>
+      <formula>$F50="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:I26">
+  <conditionalFormatting sqref="E50">
     <cfRule type="expression" dxfId="33" priority="1">
-      <formula>$F26="Fail"</formula>
+      <formula>$F50="Fail"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="32" priority="2">
-      <formula>$F26="Pass"</formula>
+      <formula>$F50="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{C71B1A12-BA98-495F-B59D-B03CB09CCB43}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{C71B1A12-BA98-495F-B59D-B03CB09CCB43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3651,14 +4406,14 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -3670,13 +4425,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="8"/>
     </row>
@@ -3685,46 +4440,46 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5">
         <f>COUNTIF(F:F,"Pass")</f>
         <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF(F:F,"Fail")</f>
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(F:F,"Not Started")</f>
@@ -3736,34 +4491,34 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
         <v>77</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>78</v>
-      </c>
-      <c r="I8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -3778,25 +4533,25 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -3805,25 +4560,25 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -3832,13 +4587,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -3847,10 +4602,10 @@
         <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -3863,7 +4618,7 @@
         <v>1010101523</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E13" s="18">
         <v>1010101523</v>
@@ -3879,13 +4634,13 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -3898,13 +4653,13 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -3917,13 +4672,13 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -3935,28 +4690,28 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3964,28 +4719,28 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3993,34 +4748,34 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -4035,13 +4790,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
@@ -4056,16 +4811,16 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>40</v>
@@ -4079,13 +4834,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
@@ -4263,7 +5018,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -4278,25 +5033,25 @@
         <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I36" s="2"/>
     </row>
@@ -4305,13 +5060,13 @@
         <v>29</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="18">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E37" s="18">
         <v>0</v>
@@ -4320,13 +5075,13 @@
         <v>37</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4334,25 +5089,25 @@
         <v>30</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I38" s="2"/>
     </row>
@@ -4361,25 +5116,25 @@
         <v>31</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I39" s="2"/>
     </row>
@@ -4388,23 +5143,23 @@
         <v>32</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I40" s="2"/>
     </row>
@@ -4681,13 +5436,13 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
@@ -4698,13 +5453,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="8"/>
     </row>
@@ -4713,46 +5468,46 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5">
         <f>COUNTIF(F:F,"Pass")</f>
         <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF(F:F,"Fail")</f>
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(F:F,"Not Started")</f>
@@ -4764,28 +5519,28 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
         <v>77</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>78</v>
-      </c>
-      <c r="I8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4808,7 +5563,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>38</v>
@@ -4820,25 +5575,25 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -4847,28 +5602,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>